<commit_message>
Format Changes & Trade Machine Mods but imperfect
</commit_message>
<xml_diff>
--- a/data/teams.xlsx
+++ b/data/teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdash/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B6090E-AC27-5F47-AB40-5CACC52C6BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B622889B-CE57-9F48-991F-9D3D2335A7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9EF46352-91BE-A141-BCB6-20FDC7061753}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{9EF46352-91BE-A141-BCB6-20FDC7061753}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,30 +168,9 @@
     <t>#BBE0FB</t>
   </si>
   <si>
-    <t>graphics/teamlogos/AFL.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/CC.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/CRB.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/ELP.png</t>
-  </si>
-  <si>
     <t>DivLogo</t>
   </si>
   <si>
-    <t>graphics/divisionlogos/GOB.png</t>
-  </si>
-  <si>
-    <t>graphics/divisionlogos/MI.png</t>
-  </si>
-  <si>
-    <t>graphics/divisionlogos/OT.png</t>
-  </si>
-  <si>
     <t>Frankfurt Roadrunners</t>
   </si>
   <si>
@@ -213,9 +192,6 @@
     <t>#152243</t>
   </si>
   <si>
-    <t>graphics/teamlogos/FRR.png</t>
-  </si>
-  <si>
     <t>Grandville Flamingos</t>
   </si>
   <si>
@@ -243,12 +219,6 @@
     <t>#B9FDC9</t>
   </si>
   <si>
-    <t>graphics/teamlogos/GF.png</t>
-  </si>
-  <si>
-    <t>graphics/divisionlogos/CH+.png</t>
-  </si>
-  <si>
     <t>Tertiary</t>
   </si>
   <si>
@@ -303,24 +273,6 @@
     <t>#FCFDFF</t>
   </si>
   <si>
-    <t>graphics/teamlogos/MCM.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/MWM.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/NN.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/VD.png</t>
-  </si>
-  <si>
-    <t>graphics/teamlogos/WLW.png</t>
-  </si>
-  <si>
-    <t>Michael Pozsar, Nico Pozsar</t>
-  </si>
-  <si>
     <t>Louie Rogers</t>
   </si>
   <si>
@@ -531,9 +483,6 @@
     <t>Madison Muskellunge</t>
   </si>
   <si>
-    <t>Charlie Moore</t>
-  </si>
-  <si>
     <t>Madison, WI</t>
   </si>
   <si>
@@ -552,9 +501,6 @@
     <t>#FFB612</t>
   </si>
   <si>
-    <t>graphics/teamlogos/MAM.png</t>
-  </si>
-  <si>
     <t>#203731</t>
   </si>
   <si>
@@ -565,6 +511,60 @@
   </si>
   <si>
     <t>#2D6642</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/AFL.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/CC.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/CRB.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/FRR.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/GF.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/MAM.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/MCM.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/MWM.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/NN.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/VD.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/WLW.png</t>
+  </si>
+  <si>
+    <t>www/graphics/divisionlogos/GOB.png</t>
+  </si>
+  <si>
+    <t>www/graphics/divisionlogos/MI.png</t>
+  </si>
+  <si>
+    <t>www/graphics/divisionlogos/OT.png</t>
+  </si>
+  <si>
+    <t>www/graphics/divisionlogos/CH+.png</t>
+  </si>
+  <si>
+    <t>www/graphics/teamlogos/ELP.png</t>
+  </si>
+  <si>
+    <t>Charlie Moore, Matt Colon</t>
+  </si>
+  <si>
+    <t>Michael, Nico &amp; Zach Pozsar</t>
   </si>
 </sst>
 </file>
@@ -920,7 +920,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,7 +937,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -967,25 +967,25 @@
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="L1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="M1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="N1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="O1" t="s">
         <v>2</v>
       </c>
       <c r="P1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1023,22 +1023,22 @@
         <v>36</v>
       </c>
       <c r="L2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" t="s">
         <v>129</v>
       </c>
-      <c r="M2" t="s">
-        <v>145</v>
-      </c>
       <c r="N2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="P2" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="Q2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1073,25 +1073,25 @@
         <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
+        <v>114</v>
+      </c>
+      <c r="M3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N3" t="s">
         <v>130</v>
       </c>
-      <c r="M3" t="s">
-        <v>147</v>
-      </c>
-      <c r="N3" t="s">
-        <v>146</v>
-      </c>
       <c r="O3" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
       <c r="Q3" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1126,25 +1126,25 @@
         <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
         <v>35</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="Q4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1179,33 +1179,33 @@
         <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" t="s">
         <v>132</v>
       </c>
-      <c r="M5" t="s">
-        <v>149</v>
-      </c>
-      <c r="N5" t="s">
-        <v>148</v>
-      </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="P5" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
       <c r="Q5" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -1214,104 +1214,104 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H6">
         <v>2015</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="M6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="N6" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
       <c r="P6" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="Q6" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H7">
         <v>2020</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="M7" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="N7" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
       <c r="P7" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="Q7" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1320,51 +1320,51 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H8">
         <v>2021</v>
       </c>
       <c r="I8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" t="s">
+        <v>156</v>
+      </c>
+      <c r="L8" t="s">
+        <v>114</v>
+      </c>
+      <c r="M8" t="s">
+        <v>158</v>
+      </c>
+      <c r="N8" t="s">
+        <v>157</v>
+      </c>
+      <c r="O8" t="s">
+        <v>164</v>
+      </c>
+      <c r="P8" t="s">
         <v>171</v>
       </c>
-      <c r="J8" t="s">
-        <v>173</v>
-      </c>
-      <c r="K8" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" t="s">
-        <v>130</v>
-      </c>
-      <c r="M8" t="s">
-        <v>176</v>
-      </c>
-      <c r="N8" t="s">
-        <v>175</v>
-      </c>
-      <c r="O8" t="s">
-        <v>172</v>
-      </c>
-      <c r="P8" t="s">
-        <v>50</v>
-      </c>
       <c r="Q8" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -1373,13 +1373,13 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H9">
         <v>2015</v>
@@ -1388,36 +1388,36 @@
         <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="L9" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="M9" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="N9" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="P9" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="Q9" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -1426,104 +1426,104 @@
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="H10">
         <v>2015</v>
       </c>
       <c r="I10" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="M10" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="N10" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="O10" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="P10" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="Q10" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" t="s">
-        <v>99</v>
-      </c>
       <c r="G11" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H11">
         <v>2020</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="J11" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="L11" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="M11" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="N11" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="O11" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="P11" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="Q11" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -1532,96 +1532,96 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="H12">
         <v>2015</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="K12" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="L12" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="M12" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="N12" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="O12" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="P12" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="Q12" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="H13">
         <v>2020</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="J13" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="K13" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="L13" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="M13" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="N13" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="O13" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="P13" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="Q13" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Everything now links off the little team icons to CBS
</commit_message>
<xml_diff>
--- a/data/teams.xlsx
+++ b/data/teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B622889B-CE57-9F48-991F-9D3D2335A7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCAB6D2-28F4-8C46-ACA6-10B5C0F3B471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{9EF46352-91BE-A141-BCB6-20FDC7061753}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="178">
   <si>
     <t>Primary</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>Michael, Nico &amp; Zach Pozsar</t>
+  </si>
+  <si>
+    <t>TeamNum</t>
   </si>
 </sst>
 </file>
@@ -917,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C474972-47A1-594C-8523-65040736B8E3}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +938,7 @@
     <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -987,8 +990,11 @@
       <c r="Q1" t="s">
         <v>100</v>
       </c>
+      <c r="R1" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1040,8 +1046,11 @@
       <c r="Q2" t="s">
         <v>110</v>
       </c>
+      <c r="R2">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1093,8 +1102,11 @@
       <c r="Q3" t="s">
         <v>106</v>
       </c>
+      <c r="R3">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1146,8 +1158,11 @@
       <c r="Q4" t="s">
         <v>103</v>
       </c>
+      <c r="R4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1199,8 +1214,11 @@
       <c r="Q5" t="s">
         <v>107</v>
       </c>
+      <c r="R5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1252,8 +1270,11 @@
       <c r="Q6" t="s">
         <v>105</v>
       </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1305,8 +1326,11 @@
       <c r="Q7" t="s">
         <v>104</v>
       </c>
+      <c r="R7">
+        <v>14</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -1358,8 +1382,11 @@
       <c r="Q8" t="s">
         <v>152</v>
       </c>
+      <c r="R8">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -1411,8 +1438,11 @@
       <c r="Q9" t="s">
         <v>108</v>
       </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1464,8 +1494,11 @@
       <c r="Q10" t="s">
         <v>153</v>
       </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1517,8 +1550,11 @@
       <c r="Q11" t="s">
         <v>102</v>
       </c>
+      <c r="R11">
+        <v>15</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1570,8 +1606,11 @@
       <c r="Q12" t="s">
         <v>101</v>
       </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -1622,6 +1661,9 @@
       </c>
       <c r="Q13" t="s">
         <v>109</v>
+      </c>
+      <c r="R13">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">

</xml_diff>